<commit_message>
Added the list of variables
</commit_message>
<xml_diff>
--- a/PCA 2011/Sumary PCA 2011.xlsx
+++ b/PCA 2011/Sumary PCA 2011.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="9465" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>District</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>No of HH's</t>
+  </si>
+  <si>
+    <t>Total Area</t>
+  </si>
+  <si>
+    <t>Proportion of crop area1</t>
+  </si>
+  <si>
+    <t>Proportion of crop area2</t>
+  </si>
+  <si>
+    <t>Proportion of crop area3</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1950,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2423,12 +2435,208 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A4:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>1/A5</f>
+        <v>0.25</v>
+      </c>
+      <c r="C5">
+        <f>2/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <f>1/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="E5">
+        <f>B5*B5</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:G8" si="0">C5*C5</f>
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H5">
+        <f>SUM(E5:G5)</f>
+        <v>0.375</v>
+      </c>
+      <c r="I5">
+        <f>1-H5</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>3/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="C6">
+        <f>1/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f>B6*B6</f>
+        <v>0.5625</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f>SUM(E6:G6)</f>
+        <v>0.625</v>
+      </c>
+      <c r="I6" s="1">
+        <f>1-H6</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f>B7*B7</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SUM(E7:G7)</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" ref="I7:I8" si="1">1-H7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>0.75</v>
+      </c>
+      <c r="C8">
+        <v>0.125</v>
+      </c>
+      <c r="D8">
+        <v>0.125</v>
+      </c>
+      <c r="E8" s="1">
+        <f>B8*B8</f>
+        <v>0.5625</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUM(E8:G8)</f>
+        <v>0.59375</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <f>B9*B9</f>
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" ref="F9" si="2">C9*C9</f>
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" ref="G9" si="3">D9*D9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SUM(E9:G9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" ref="I9" si="4">1-H9</f>
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>